<commit_message>
USB2 read daten anstatt USB3
</commit_message>
<xml_diff>
--- a/Uebung_SPCundVarianzanalyse/Michael_Schulze.xlsx
+++ b/Uebung_SPCundVarianzanalyse/Michael_Schulze.xlsx
@@ -21,14 +21,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,19 +90,23 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -110,71 +116,84 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
-        <v>156.483</v>
+        <v>17.387</v>
       </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>152.646</v>
+        <v>16.96</v>
       </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>158.7517</v>
+        <v>17.639</v>
       </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>149.832</v>
+        <v>16.648</v>
       </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>166.877</v>
+        <v>18.541</v>
       </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>162.222</v>
+        <v>18.024</v>
       </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>166.983</v>
+        <v>18.553</v>
       </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>159.079</v>
+        <v>17.675</v>
       </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>163.522</v>
+        <v>18.169</v>
       </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>150.724</v>
+        <v>16.747</v>
       </c>
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>